<commit_message>
working version, w/ dropdowns... add more charts tomorrow
</commit_message>
<xml_diff>
--- a/decision_log.xlsx
+++ b/decision_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Allie/Workspace/revOps_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833B5E8A-1787-AA41-9D69-625163484EC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E9A581-AD2F-2846-84C4-F2998D55749B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{5012CBB8-F046-554B-AC92-AA1359997254}"/>
+    <workbookView xWindow="5800" yWindow="5880" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{5012CBB8-F046-554B-AC92-AA1359997254}"/>
   </bookViews>
   <sheets>
     <sheet name="Brainstorming" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Possible Charting Options</t>
   </si>
@@ -104,6 +104,33 @@
   </si>
   <si>
     <t>Began leveraging a simple Dash framework to get started, will expand as time allows.</t>
+  </si>
+  <si>
+    <t>Mockaroo Limitations</t>
+  </si>
+  <si>
+    <t>Limited in ability to manipulate mock datasets, so will separate opportunities from actual purchases.</t>
+  </si>
+  <si>
+    <t>Minimal - extra code that would otherwise not be required</t>
+  </si>
+  <si>
+    <t>Implemented code at onset of main app py file to merge datasets</t>
+  </si>
+  <si>
+    <t>Separate "account"/"purchase" vs "opportunity" datasets</t>
+  </si>
+  <si>
+    <t>Originally tried to condense code to include line in `app.layout` that had final line of "html.Div(id='outputDiv', children=[])" drawing from a function, but charts would not render.</t>
+  </si>
+  <si>
+    <t>Include chart codes in `app.layout`</t>
+  </si>
+  <si>
+    <t>Charts not properly rendering</t>
+  </si>
+  <si>
+    <t>Code will be less concise, and (I find) less readable</t>
   </si>
 </sst>
 </file>
@@ -590,7 +617,8 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -654,8 +682,43 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1"/>
-    <row r="6" spans="1:8" s="6" customFormat="1"/>
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="85">
+      <c r="A5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7">
+        <v>45059</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="153">
+      <c r="A6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="7">
+        <v>45060</v>
+      </c>
+    </row>
     <row r="7" spans="1:8" s="6" customFormat="1"/>
     <row r="8" spans="1:8" s="6" customFormat="1"/>
     <row r="9" spans="1:8" s="6" customFormat="1"/>

</xml_diff>

<commit_message>
test run for local deploy
</commit_message>
<xml_diff>
--- a/decision_log.xlsx
+++ b/decision_log.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Allie/Workspace/revOps_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C6ABB1-ED01-B54F-B671-00308D0813D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58AFC96-4247-2F46-820F-96A3B59335A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="3580" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{5012CBB8-F046-554B-AC92-AA1359997254}"/>
+    <workbookView xWindow="6760" yWindow="3580" windowWidth="27640" windowHeight="16940" xr2:uid="{5012CBB8-F046-554B-AC92-AA1359997254}"/>
   </bookViews>
   <sheets>
     <sheet name="Brainstorming" sheetId="1" r:id="rId1"/>
-    <sheet name="Things to Fix" sheetId="3" r:id="rId2"/>
-    <sheet name="Decision Log" sheetId="2" r:id="rId3"/>
+    <sheet name="Decision Log" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="192">
   <si>
     <t>Possible Charting Options</t>
   </si>
@@ -570,6 +569,39 @@
   </si>
   <si>
     <t>More material/impactful results</t>
+  </si>
+  <si>
+    <t>Forego win rate strip chart</t>
+  </si>
+  <si>
+    <t>Win rate strip chart getting too messy to break down by make/model. Groupbys becoming extremely time consuming. Will forego for now</t>
+  </si>
+  <si>
+    <t>Missing chart</t>
+  </si>
+  <si>
+    <t>Extreme predictions</t>
+  </si>
+  <si>
+    <t>Host on Render</t>
+  </si>
+  <si>
+    <t>Heroku no longer free</t>
+  </si>
+  <si>
+    <t>Heroku is no longer free, there is a free service called Render for Dash apps</t>
+  </si>
+  <si>
+    <t>Service will be slower</t>
+  </si>
+  <si>
+    <t>Deployed on Render successfully</t>
+  </si>
+  <si>
+    <t>Slow chart generatin</t>
+  </si>
+  <si>
+    <t>Not as precise as I would like, but it works.</t>
   </si>
 </sst>
 </file>
@@ -784,7 +816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -868,7 +900,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1185,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4540EF93-91FE-C644-B2FC-CAF391A7BB93}">
   <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2667,39 +2698,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8408108-C917-1848-B277-1E0F02485ED6}">
-  <dimension ref="A2:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="54.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2" s="35"/>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="35"/>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="35"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E274BF97-3904-BF42-ABA8-CA221B553A5D}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3084,6 +3088,9 @@
       <c r="F17" s="5" t="s">
         <v>146</v>
       </c>
+      <c r="G17" s="5" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1" ht="119">
       <c r="A18" s="5" t="s">
@@ -3127,6 +3134,9 @@
       <c r="F19" s="5" t="s">
         <v>170</v>
       </c>
+      <c r="G19" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="20" spans="1:7" s="5" customFormat="1" ht="102">
       <c r="A20" s="5" t="s">
@@ -3171,8 +3181,46 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1"/>
-    <row r="23" spans="1:7" s="5" customFormat="1"/>
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="102">
+      <c r="A22" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E22" s="7">
+        <v>45064</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="5" customFormat="1" ht="51">
+      <c r="A23" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E23" s="6">
+        <v>45065</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
     <row r="24" spans="1:7" s="5" customFormat="1"/>
     <row r="25" spans="1:7" s="5" customFormat="1"/>
     <row r="26" spans="1:7" s="5" customFormat="1"/>

</xml_diff>